<commit_message>
cambio de documento 03_INDICADORES_DE_RESULTADOS tercer trimestre 2024
</commit_message>
<xml_diff>
--- a/src/assets/content/estados-financieros/2024/tercer-trimestre/03_INFORMACION_PROGRAMATICA/03_INDICADORES_DE_RESULTADOS.xlsx
+++ b/src/assets/content/estados-financieros/2024/tercer-trimestre/03_INFORMACION_PROGRAMATICA/03_INDICADORES_DE_RESULTADOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utsalamancaedu-my.sharepoint.com/personal/zcampos_utsalamanca_edu_mx/Documents/1.-EJERCICIO 2024/3.- 3ER TRIMESTRE/SIRET/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utsalamancaedu-my.sharepoint.com/personal/zcampos_utsalamanca_edu_mx/Documents/1.-EJERCICIO 2024/3.- 3ER TRIMESTRE/PUBLICACION EN LA PAGINA UTS/4_INFORMACION DE POSTURA FISCAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C10C7C03-1337-4FC9-867C-E2ADE6D8C351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{C10C7C03-1337-4FC9-867C-E2ADE6D8C351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C566082D-C369-4209-BB51-1262F8665E87}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,13 +541,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="General_)"/>
+    <numFmt numFmtId="165" formatCode="General_)"/>
   </numFmts>
   <fonts count="55" x14ac:knownFonts="1">
     <font>
@@ -1543,81 +1541,81 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -1710,18 +1708,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="19" fillId="23" borderId="9" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1837,17 +1835,17 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2761,15 +2759,15 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2782,29 +2780,29 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2812,82 +2810,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2977,6 +2975,41 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -2986,41 +3019,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -4284,9 +4282,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -4309,32 +4310,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="30"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="40"/>
     </row>
     <row r="2" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
@@ -4447,890 +4448,890 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="31">
         <v>22359697.32</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="31">
         <v>27424413.75</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I4" s="31">
         <v>108577.49</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4" s="31">
         <v>13455543.560000001</v>
       </c>
-      <c r="K4" s="34">
+      <c r="K4" s="31">
         <v>9682734.3599999994</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N4" s="36" t="s">
+      <c r="N4" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="O4" s="36" t="s">
+      <c r="O4" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="P4" s="35" t="s">
+      <c r="P4" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R4" s="37" t="s">
+      <c r="R4" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="S4" s="38">
+      <c r="S4" s="35">
         <v>2100</v>
       </c>
-      <c r="T4" s="38" t="s">
+      <c r="T4" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U4" s="38">
+      <c r="U4" s="35">
         <v>1999</v>
       </c>
-      <c r="V4" s="38">
+      <c r="V4" s="35">
         <v>1999</v>
       </c>
-      <c r="W4" s="38">
+      <c r="W4" s="35">
         <v>2100</v>
       </c>
-      <c r="X4" s="36" t="s">
+      <c r="X4" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="31">
         <v>3689425.98</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="31">
         <v>4286694.51</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="31">
         <v>113252.19</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="31">
         <v>2160455.36</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="31">
         <v>2047203.17</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="L5" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="M5" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q5" s="37" t="s">
+      <c r="Q5" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R5" s="37" t="s">
+      <c r="R5" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="S5" s="38">
+      <c r="S5" s="35">
         <v>4</v>
       </c>
-      <c r="T5" s="38" t="s">
+      <c r="T5" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U5" s="38" t="s">
+      <c r="U5" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="V5" s="38" t="s">
+      <c r="V5" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="W5" s="38">
+      <c r="W5" s="35">
         <v>4</v>
       </c>
-      <c r="X5" s="36" t="s">
+      <c r="X5" s="33" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="31">
         <v>1873016.39</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="31">
         <v>1957681.45</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="31">
         <v>0</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="31">
         <v>9749.56</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="31">
         <v>9749.56</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M6" s="35" t="s">
+      <c r="M6" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N6" s="36" t="s">
+      <c r="N6" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="O6" s="36" t="s">
+      <c r="O6" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q6" s="37" t="s">
+      <c r="Q6" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R6" s="37" t="s">
+      <c r="R6" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="S6" s="38">
+      <c r="S6" s="35">
         <v>1293</v>
       </c>
-      <c r="T6" s="38" t="s">
+      <c r="T6" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U6" s="38">
+      <c r="U6" s="35">
         <v>1002</v>
       </c>
-      <c r="V6" s="38">
+      <c r="V6" s="35">
         <v>1002</v>
       </c>
-      <c r="W6" s="38">
+      <c r="W6" s="35">
         <v>1293</v>
       </c>
-      <c r="X6" s="36" t="s">
+      <c r="X6" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="31">
         <v>462697.08</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="31">
         <v>483861.34</v>
       </c>
-      <c r="I7" s="34">
+      <c r="I7" s="31">
         <v>0</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="31">
         <v>19308.11</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="31">
         <v>19308.11</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="L7" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="35" t="s">
+      <c r="M7" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N7" s="36" t="s">
+      <c r="N7" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="O7" s="36" t="s">
+      <c r="O7" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q7" s="37" t="s">
+      <c r="Q7" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R7" s="37" t="s">
+      <c r="R7" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="S7" s="38">
+      <c r="S7" s="35">
         <v>2100</v>
       </c>
-      <c r="T7" s="38" t="s">
+      <c r="T7" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U7" s="38" t="s">
+      <c r="U7" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="V7" s="38" t="s">
+      <c r="V7" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="W7" s="38">
+      <c r="W7" s="35">
         <v>2100</v>
       </c>
-      <c r="X7" s="36" t="s">
+      <c r="X7" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="66" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="31">
         <v>462697.08</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="31">
         <v>483861.34</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="31">
         <v>0</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="31">
         <v>19308.11</v>
       </c>
-      <c r="K8" s="34">
+      <c r="K8" s="31">
         <v>19308.11</v>
       </c>
-      <c r="L8" s="35" t="s">
+      <c r="L8" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M8" s="35" t="s">
+      <c r="M8" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N8" s="36" t="s">
+      <c r="N8" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="O8" s="36" t="s">
+      <c r="O8" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q8" s="37" t="s">
+      <c r="Q8" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="37" t="s">
+      <c r="R8" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="S8" s="38">
+      <c r="S8" s="35">
         <v>56</v>
       </c>
-      <c r="T8" s="38" t="s">
+      <c r="T8" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U8" s="38" t="s">
+      <c r="U8" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="V8" s="38" t="s">
+      <c r="V8" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="W8" s="38">
+      <c r="W8" s="35">
         <v>56</v>
       </c>
-      <c r="X8" s="36" t="s">
+      <c r="X8" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="31">
         <v>991008.15</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="31">
         <v>1033340.69</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="31">
         <v>0</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="31">
         <v>27920.97</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="31">
         <v>27920.97</v>
       </c>
-      <c r="L9" s="35" t="s">
+      <c r="L9" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="35" t="s">
+      <c r="M9" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="N9" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="O9" s="36" t="s">
+      <c r="O9" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="P9" s="35" t="s">
+      <c r="P9" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q9" s="37" t="s">
+      <c r="Q9" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R9" s="37" t="s">
+      <c r="R9" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="S9" s="38">
+      <c r="S9" s="35">
         <v>80</v>
       </c>
-      <c r="T9" s="38" t="s">
+      <c r="T9" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U9" s="38" t="s">
+      <c r="U9" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="V9" s="38" t="s">
+      <c r="V9" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="W9" s="38">
+      <c r="W9" s="35">
         <v>80</v>
       </c>
-      <c r="X9" s="36" t="s">
+      <c r="X9" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="31">
         <v>2306653.64</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="31">
         <v>2327819.9</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="31">
         <v>374532</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="31">
         <v>712681.25</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10" s="31">
         <v>338149.25</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="M10" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N10" s="36" t="s">
+      <c r="N10" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="O10" s="36" t="s">
+      <c r="O10" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="P10" s="35" t="s">
+      <c r="P10" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q10" s="37" t="s">
+      <c r="Q10" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="R10" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="S10" s="38">
+      <c r="S10" s="35">
         <v>382</v>
       </c>
-      <c r="T10" s="38" t="s">
+      <c r="T10" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U10" s="38">
+      <c r="U10" s="35">
         <v>310</v>
       </c>
-      <c r="V10" s="38">
+      <c r="V10" s="35">
         <v>310</v>
       </c>
-      <c r="W10" s="38">
+      <c r="W10" s="35">
         <v>382</v>
       </c>
-      <c r="X10" s="36" t="s">
+      <c r="X10" s="33" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="66" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="31">
         <v>525504.07999999996</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="31">
         <v>546670.34</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="31">
         <v>64391</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="31">
         <v>124817.95</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="31">
         <v>60426.95</v>
       </c>
-      <c r="L11" s="35" t="s">
+      <c r="L11" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M11" s="35" t="s">
+      <c r="M11" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N11" s="36" t="s">
+      <c r="N11" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="O11" s="36" t="s">
+      <c r="O11" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="P11" s="35" t="s">
+      <c r="P11" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q11" s="37" t="s">
+      <c r="Q11" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R11" s="37" t="s">
+      <c r="R11" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="S11" s="38">
+      <c r="S11" s="35">
         <v>1650</v>
       </c>
-      <c r="T11" s="38" t="s">
+      <c r="T11" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U11" s="38">
+      <c r="U11" s="35">
         <v>766</v>
       </c>
-      <c r="V11" s="38">
+      <c r="V11" s="35">
         <v>766</v>
       </c>
-      <c r="W11" s="38">
+      <c r="W11" s="35">
         <v>1650</v>
       </c>
-      <c r="X11" s="36" t="s">
+      <c r="X11" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="31">
         <v>3949536.83</v>
       </c>
-      <c r="H12" s="34">
+      <c r="H12" s="31">
         <v>4140033.27</v>
       </c>
-      <c r="I12" s="34">
+      <c r="I12" s="31">
         <v>0</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="31">
         <v>1012464.45</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12" s="31">
         <v>1012464.45</v>
       </c>
-      <c r="L12" s="35" t="s">
+      <c r="L12" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M12" s="35" t="s">
+      <c r="M12" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N12" s="36" t="s">
+      <c r="N12" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="O12" s="36" t="s">
+      <c r="O12" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="P12" s="35" t="s">
+      <c r="P12" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q12" s="37" t="s">
+      <c r="Q12" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R12" s="37" t="s">
+      <c r="R12" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="S12" s="38">
+      <c r="S12" s="35">
         <v>2</v>
       </c>
-      <c r="T12" s="38" t="s">
+      <c r="T12" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U12" s="38">
+      <c r="U12" s="35">
         <v>1</v>
       </c>
-      <c r="V12" s="38">
+      <c r="V12" s="35">
         <v>1</v>
       </c>
-      <c r="W12" s="38">
+      <c r="W12" s="35">
         <v>2</v>
       </c>
-      <c r="X12" s="36" t="s">
+      <c r="X12" s="33" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="31">
         <v>504504.08</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="31">
         <v>525670.34</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="31">
         <v>0</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="31">
         <v>0</v>
       </c>
-      <c r="K13" s="34">
+      <c r="K13" s="31">
         <v>0</v>
       </c>
-      <c r="L13" s="35" t="s">
+      <c r="L13" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M13" s="35" t="s">
+      <c r="M13" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N13" s="36" t="s">
+      <c r="N13" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="O13" s="36" t="s">
+      <c r="O13" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="P13" s="35" t="s">
+      <c r="P13" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q13" s="37" t="s">
+      <c r="Q13" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R13" s="37" t="s">
+      <c r="R13" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="S13" s="38">
+      <c r="S13" s="35">
         <v>1</v>
       </c>
-      <c r="T13" s="38" t="s">
+      <c r="T13" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U13" s="38">
+      <c r="U13" s="35">
         <v>1</v>
       </c>
-      <c r="V13" s="38">
+      <c r="V13" s="35">
         <v>1</v>
       </c>
-      <c r="W13" s="38">
+      <c r="W13" s="35">
         <v>1</v>
       </c>
-      <c r="X13" s="36" t="s">
+      <c r="X13" s="33" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="31">
         <v>625504.07999999996</v>
       </c>
-      <c r="H14" s="34">
+      <c r="H14" s="31">
         <v>646670.34</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="31">
         <v>0</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="31">
         <v>116171.73</v>
       </c>
-      <c r="K14" s="34">
+      <c r="K14" s="31">
         <v>116171.73</v>
       </c>
-      <c r="L14" s="35" t="s">
+      <c r="L14" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M14" s="35" t="s">
+      <c r="M14" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N14" s="36" t="s">
+      <c r="N14" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="O14" s="36" t="s">
+      <c r="O14" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="P14" s="35" t="s">
+      <c r="P14" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q14" s="37" t="s">
+      <c r="Q14" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R14" s="37" t="s">
+      <c r="R14" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="S14" s="38">
+      <c r="S14" s="35">
         <v>95</v>
       </c>
-      <c r="T14" s="38" t="s">
+      <c r="T14" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U14" s="38" t="s">
+      <c r="U14" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="V14" s="38" t="s">
+      <c r="V14" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="W14" s="38">
+      <c r="W14" s="35">
         <v>95</v>
       </c>
-      <c r="X14" s="36" t="s">
+      <c r="X14" s="33" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="31">
         <v>2613327.4500000002</v>
       </c>
-      <c r="H15" s="34">
+      <c r="H15" s="31">
         <v>2719158.83</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="31">
         <v>132870.78</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="31">
         <v>440178.4</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="31">
         <v>299763.55</v>
       </c>
-      <c r="L15" s="35" t="s">
+      <c r="L15" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M15" s="35" t="s">
+      <c r="M15" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N15" s="36" t="s">
+      <c r="N15" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="O15" s="36" t="s">
+      <c r="O15" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="P15" s="35" t="s">
+      <c r="P15" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q15" s="37" t="s">
+      <c r="Q15" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R15" s="37" t="s">
+      <c r="R15" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="S15" s="38">
+      <c r="S15" s="35">
         <v>2100</v>
       </c>
-      <c r="T15" s="38" t="s">
+      <c r="T15" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="U15" s="38">
+      <c r="U15" s="35">
         <v>1228</v>
       </c>
-      <c r="V15" s="38">
+      <c r="V15" s="35">
         <v>1228</v>
       </c>
-      <c r="W15" s="38">
+      <c r="W15" s="35">
         <v>2100</v>
       </c>
-      <c r="X15" s="36" t="s">
+      <c r="X15" s="33" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5467,8 +5468,8 @@
   <mergeCells count="1">
     <mergeCell ref="A1:X1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="28" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5934,6 +5935,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100828CC21759168C4EAD7644AD10074825" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="36610a04559c883f4218115f04267619">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b2b1fa7a59e354d7f595b7732424404">
     <xsd:element name="properties">
@@ -6047,12 +6054,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F51EF88-68BC-4A76-B5D9-47B8734FF48E}">
   <ds:schemaRefs>
@@ -6062,6 +6063,21 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDF2C03A-FAFE-4FBB-9F24-298C907734CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DADBACD-142E-411B-8495-70B1A186C30D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6075,19 +6091,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDF2C03A-FAFE-4FBB-9F24-298C907734CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>